<commit_message>
admin all module number 1 to n, student/faculty file import success-bugs solved,
</commit_message>
<xml_diff>
--- a/Sample Data File/Faculty_OriginalData.xlsx
+++ b/Sample Data File/Faculty_OriginalData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RDBMS\ARP DATA\Data Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\arp_\Sample Data File\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A5EF3E-057A-4E71-9DB9-9C6C34EA0489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11DB167A-C94F-4BEB-AE01-76B87C897B98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{7D3FE9B7-6610-42F8-BCFA-F1D64A857B15}"/>
   </bookViews>
@@ -500,7 +500,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -508,16 +508,13 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -856,8 +853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15E31926-3C60-444F-9410-D832235ADECD}">
   <dimension ref="A1:E119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A120" sqref="A120:XFD148"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -868,19 +865,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -888,16 +885,16 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <v>220925</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>126</v>
       </c>
     </row>
@@ -905,16 +902,16 @@
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>789012</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>128</v>
       </c>
     </row>
@@ -922,16 +919,16 @@
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>316632</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="D4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -939,16 +936,16 @@
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>316261</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="D5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>127</v>
       </c>
     </row>
@@ -956,16 +953,16 @@
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>316448</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="D6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>129</v>
       </c>
     </row>
@@ -973,16 +970,16 @@
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>316519</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="D7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>130</v>
       </c>
     </row>
@@ -990,16 +987,16 @@
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>315906</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="D8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>132</v>
       </c>
     </row>
@@ -1007,16 +1004,16 @@
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>311787</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E9" s="3" t="s">
+      <c r="D9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>131</v>
       </c>
     </row>
@@ -1024,13 +1021,13 @@
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <v>315297</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="2" t="s">
@@ -1041,13 +1038,13 @@
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <v>312818</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="2" t="s">
@@ -1058,13 +1055,13 @@
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="5">
         <v>313137</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="2" t="s">
@@ -1075,16 +1072,16 @@
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <v>314751</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E13" s="3" t="s">
+      <c r="D13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>126</v>
       </c>
     </row>
@@ -1092,16 +1089,16 @@
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="5">
         <v>312038</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E14" s="3" t="s">
+      <c r="D14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1109,16 +1106,16 @@
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="5">
         <v>315760</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E15" s="3" t="s">
+      <c r="D15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1126,16 +1123,16 @@
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="5">
         <v>316046</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E16" s="3" t="s">
+      <c r="D16" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1143,16 +1140,16 @@
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="5">
         <v>315762</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E17" s="3" t="s">
+      <c r="D17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>129</v>
       </c>
     </row>
@@ -1160,16 +1157,16 @@
       <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="5">
         <v>314143</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E18" s="3" t="s">
+      <c r="D18" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>130</v>
       </c>
     </row>
@@ -1177,16 +1174,16 @@
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="5">
         <v>315756</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E19" s="3" t="s">
+      <c r="D19" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>132</v>
       </c>
     </row>
@@ -1194,16 +1191,16 @@
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="5">
         <v>316022</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E20" s="3" t="s">
+      <c r="D20" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>131</v>
       </c>
     </row>
@@ -1211,13 +1208,13 @@
       <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="5">
         <v>315295</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E21" s="2" t="s">
@@ -1228,13 +1225,13 @@
       <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="5">
         <v>315617</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E22" s="2" t="s">
@@ -1245,13 +1242,13 @@
       <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="5">
         <v>315769</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E23" s="2" t="s">
@@ -1262,16 +1259,16 @@
       <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="5">
         <v>312777</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E24" s="3" t="s">
+      <c r="D24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>126</v>
       </c>
     </row>
@@ -1279,16 +1276,16 @@
       <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="5">
         <v>316794</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E25" s="3" t="s">
+      <c r="D25" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1296,16 +1293,16 @@
       <c r="A26" s="1">
         <v>25</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="5">
         <v>316003</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E26" s="3" t="s">
+      <c r="D26" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1313,16 +1310,16 @@
       <c r="A27" s="1">
         <v>26</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="5">
         <v>316001</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D27" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E27" s="3" t="s">
+      <c r="D27" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1330,16 +1327,16 @@
       <c r="A28" s="1">
         <v>27</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="5">
         <v>314664</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D28" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E28" s="3" t="s">
+      <c r="D28" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>129</v>
       </c>
     </row>
@@ -1347,16 +1344,16 @@
       <c r="A29" s="1">
         <v>28</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B29" s="5">
         <v>313284</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D29" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E29" s="3" t="s">
+      <c r="D29" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>130</v>
       </c>
     </row>
@@ -1364,16 +1361,16 @@
       <c r="A30" s="1">
         <v>29</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B30" s="5">
         <v>316316</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D30" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E30" s="3" t="s">
+      <c r="D30" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>132</v>
       </c>
     </row>
@@ -1381,16 +1378,16 @@
       <c r="A31" s="1">
         <v>30</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31" s="5">
         <v>315430</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D31" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E31" s="3" t="s">
+      <c r="D31" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>131</v>
       </c>
     </row>
@@ -1398,13 +1395,13 @@
       <c r="A32" s="1">
         <v>31</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B32" s="5">
         <v>311034</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E32" s="2" t="s">
@@ -1415,13 +1412,13 @@
       <c r="A33" s="1">
         <v>32</v>
       </c>
-      <c r="B33" s="6">
+      <c r="B33" s="5">
         <v>315318</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C33" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E33" s="2" t="s">
@@ -1432,13 +1429,13 @@
       <c r="A34" s="1">
         <v>33</v>
       </c>
-      <c r="B34" s="6">
+      <c r="B34" s="5">
         <v>314728</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E34" s="2" t="s">
@@ -1449,16 +1446,16 @@
       <c r="A35" s="1">
         <v>34</v>
       </c>
-      <c r="B35" s="6">
+      <c r="B35" s="5">
         <v>312819</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D35" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E35" s="3" t="s">
+      <c r="D35" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>126</v>
       </c>
     </row>
@@ -1466,16 +1463,16 @@
       <c r="A36" s="1">
         <v>35</v>
       </c>
-      <c r="B36" s="6">
+      <c r="B36" s="5">
         <v>316876</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D36" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E36" s="3" t="s">
+      <c r="D36" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1483,16 +1480,16 @@
       <c r="A37" s="1">
         <v>36</v>
       </c>
-      <c r="B37" s="6">
+      <c r="B37" s="5">
         <v>315494</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D37" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E37" s="3" t="s">
+      <c r="D37" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1500,16 +1497,16 @@
       <c r="A38" s="1">
         <v>37</v>
       </c>
-      <c r="B38" s="6">
+      <c r="B38" s="5">
         <v>315157</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D38" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E38" s="3" t="s">
+      <c r="D38" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1517,16 +1514,16 @@
       <c r="A39" s="1">
         <v>38</v>
       </c>
-      <c r="B39" s="6">
+      <c r="B39" s="5">
         <v>312176</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C39" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D39" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E39" s="3" t="s">
+      <c r="D39" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>129</v>
       </c>
     </row>
@@ -1534,16 +1531,16 @@
       <c r="A40" s="1">
         <v>39</v>
       </c>
-      <c r="B40" s="6">
+      <c r="B40" s="5">
         <v>312024</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C40" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D40" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E40" s="3" t="s">
+      <c r="D40" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>130</v>
       </c>
     </row>
@@ -1551,16 +1548,16 @@
       <c r="A41" s="1">
         <v>40</v>
       </c>
-      <c r="B41" s="6">
+      <c r="B41" s="5">
         <v>314663</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C41" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D41" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E41" s="3" t="s">
+      <c r="D41" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E41" s="2" t="s">
         <v>132</v>
       </c>
     </row>
@@ -1568,16 +1565,16 @@
       <c r="A42" s="1">
         <v>41</v>
       </c>
-      <c r="B42" s="6">
+      <c r="B42" s="5">
         <v>315758</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C42" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D42" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E42" s="3" t="s">
+      <c r="D42" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E42" s="2" t="s">
         <v>131</v>
       </c>
     </row>
@@ -1585,13 +1582,13 @@
       <c r="A43" s="1">
         <v>42</v>
       </c>
-      <c r="B43" s="6">
+      <c r="B43" s="5">
         <v>314436</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C43" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="D43" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E43" s="2" t="s">
@@ -1602,13 +1599,13 @@
       <c r="A44" s="1">
         <v>43</v>
       </c>
-      <c r="B44" s="6">
+      <c r="B44" s="5">
         <v>316175</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="C44" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="D44" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E44" s="2" t="s">
@@ -1619,13 +1616,13 @@
       <c r="A45" s="1">
         <v>44</v>
       </c>
-      <c r="B45" s="6">
+      <c r="B45" s="5">
         <v>314304</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C45" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D45" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E45" s="2" t="s">
@@ -1636,16 +1633,16 @@
       <c r="A46" s="1">
         <v>45</v>
       </c>
-      <c r="B46" s="6">
+      <c r="B46" s="5">
         <v>311764</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C46" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D46" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E46" s="3" t="s">
+      <c r="D46" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>126</v>
       </c>
     </row>
@@ -1653,16 +1650,16 @@
       <c r="A47" s="1">
         <v>46</v>
       </c>
-      <c r="B47" s="6">
+      <c r="B47" s="5">
         <v>316179</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="C47" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D47" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E47" s="3" t="s">
+      <c r="D47" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1670,16 +1667,16 @@
       <c r="A48" s="1">
         <v>47</v>
       </c>
-      <c r="B48" s="6">
+      <c r="B48" s="5">
         <v>315814</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="C48" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D48" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E48" s="3" t="s">
+      <c r="D48" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E48" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1687,16 +1684,16 @@
       <c r="A49" s="1">
         <v>48</v>
       </c>
-      <c r="B49" s="6">
+      <c r="B49" s="5">
         <v>314776</v>
       </c>
-      <c r="C49" s="6" t="s">
+      <c r="C49" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D49" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E49" s="3" t="s">
+      <c r="D49" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E49" s="2" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1704,16 +1701,16 @@
       <c r="A50" s="1">
         <v>49</v>
       </c>
-      <c r="B50" s="6">
+      <c r="B50" s="5">
         <v>316025</v>
       </c>
-      <c r="C50" s="6" t="s">
+      <c r="C50" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D50" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E50" s="3" t="s">
+      <c r="D50" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E50" s="2" t="s">
         <v>129</v>
       </c>
     </row>
@@ -1721,16 +1718,16 @@
       <c r="A51" s="1">
         <v>50</v>
       </c>
-      <c r="B51" s="6">
+      <c r="B51" s="5">
         <v>316317</v>
       </c>
-      <c r="C51" s="6" t="s">
+      <c r="C51" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D51" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E51" s="3" t="s">
+      <c r="D51" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E51" s="2" t="s">
         <v>130</v>
       </c>
     </row>
@@ -1738,16 +1735,16 @@
       <c r="A52" s="1">
         <v>51</v>
       </c>
-      <c r="B52" s="6">
+      <c r="B52" s="5">
         <v>314727</v>
       </c>
-      <c r="C52" s="6" t="s">
+      <c r="C52" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D52" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E52" s="3" t="s">
+      <c r="D52" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E52" s="2" t="s">
         <v>132</v>
       </c>
     </row>
@@ -1755,16 +1752,16 @@
       <c r="A53" s="1">
         <v>52</v>
       </c>
-      <c r="B53" s="6">
+      <c r="B53" s="5">
         <v>311639</v>
       </c>
-      <c r="C53" s="6" t="s">
+      <c r="C53" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D53" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E53" s="3" t="s">
+      <c r="D53" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E53" s="2" t="s">
         <v>131</v>
       </c>
     </row>
@@ -1772,13 +1769,13 @@
       <c r="A54" s="1">
         <v>53</v>
       </c>
-      <c r="B54" s="6">
+      <c r="B54" s="5">
         <v>316004</v>
       </c>
-      <c r="C54" s="6" t="s">
+      <c r="C54" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D54" s="5" t="s">
+      <c r="D54" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E54" s="2" t="s">
@@ -1789,13 +1786,13 @@
       <c r="A55" s="1">
         <v>54</v>
       </c>
-      <c r="B55" s="6">
+      <c r="B55" s="5">
         <v>316640</v>
       </c>
-      <c r="C55" s="6" t="s">
+      <c r="C55" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="D55" s="5" t="s">
+      <c r="D55" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E55" s="2" t="s">
@@ -1806,13 +1803,13 @@
       <c r="A56" s="1">
         <v>55</v>
       </c>
-      <c r="B56" s="6">
+      <c r="B56" s="5">
         <v>312054</v>
       </c>
-      <c r="C56" s="6" t="s">
+      <c r="C56" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D56" s="5" t="s">
+      <c r="D56" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E56" s="2" t="s">
@@ -1823,16 +1820,16 @@
       <c r="A57" s="1">
         <v>56</v>
       </c>
-      <c r="B57" s="6">
+      <c r="B57" s="5">
         <v>312926</v>
       </c>
-      <c r="C57" s="6" t="s">
+      <c r="C57" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D57" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E57" s="3" t="s">
+      <c r="D57" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E57" s="2" t="s">
         <v>126</v>
       </c>
     </row>
@@ -1840,16 +1837,16 @@
       <c r="A58" s="1">
         <v>57</v>
       </c>
-      <c r="B58" s="6">
+      <c r="B58" s="5">
         <v>312180</v>
       </c>
-      <c r="C58" s="6" t="s">
+      <c r="C58" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D58" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E58" s="3" t="s">
+      <c r="D58" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E58" s="2" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1857,16 +1854,16 @@
       <c r="A59" s="1">
         <v>58</v>
       </c>
-      <c r="B59" s="6">
+      <c r="B59" s="5">
         <v>316002</v>
       </c>
-      <c r="C59" s="6" t="s">
+      <c r="C59" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D59" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E59" s="3" t="s">
+      <c r="D59" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E59" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1874,16 +1871,16 @@
       <c r="A60" s="1">
         <v>59</v>
       </c>
-      <c r="B60" s="6">
+      <c r="B60" s="5">
         <v>314142</v>
       </c>
-      <c r="C60" s="6" t="s">
+      <c r="C60" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D60" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E60" s="3" t="s">
+      <c r="D60" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E60" s="2" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1891,16 +1888,16 @@
       <c r="A61" s="1">
         <v>60</v>
       </c>
-      <c r="B61" s="6">
+      <c r="B61" s="5">
         <v>314098</v>
       </c>
-      <c r="C61" s="6" t="s">
+      <c r="C61" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D61" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E61" s="3" t="s">
+      <c r="D61" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E61" s="2" t="s">
         <v>129</v>
       </c>
     </row>
@@ -1908,16 +1905,16 @@
       <c r="A62" s="1">
         <v>61</v>
       </c>
-      <c r="B62" s="6">
+      <c r="B62" s="5">
         <v>314821</v>
       </c>
-      <c r="C62" s="6" t="s">
+      <c r="C62" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D62" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E62" s="3" t="s">
+      <c r="D62" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E62" s="2" t="s">
         <v>130</v>
       </c>
     </row>
@@ -1925,16 +1922,16 @@
       <c r="A63" s="1">
         <v>62</v>
       </c>
-      <c r="B63" s="6">
+      <c r="B63" s="5">
         <v>315815</v>
       </c>
-      <c r="C63" s="6" t="s">
+      <c r="C63" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D63" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E63" s="3" t="s">
+      <c r="D63" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E63" s="2" t="s">
         <v>132</v>
       </c>
     </row>
@@ -1942,16 +1939,16 @@
       <c r="A64" s="1">
         <v>63</v>
       </c>
-      <c r="B64" s="6">
+      <c r="B64" s="5">
         <v>316185</v>
       </c>
-      <c r="C64" s="6" t="s">
+      <c r="C64" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D64" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E64" s="3" t="s">
+      <c r="D64" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E64" s="2" t="s">
         <v>131</v>
       </c>
     </row>
@@ -1959,13 +1956,13 @@
       <c r="A65" s="1">
         <v>64</v>
       </c>
-      <c r="B65" s="6">
+      <c r="B65" s="5">
         <v>314670</v>
       </c>
-      <c r="C65" s="6" t="s">
+      <c r="C65" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D65" s="5" t="s">
+      <c r="D65" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E65" s="2" t="s">
@@ -1976,13 +1973,13 @@
       <c r="A66" s="1">
         <v>65</v>
       </c>
-      <c r="B66" s="6">
+      <c r="B66" s="5">
         <v>312031</v>
       </c>
-      <c r="C66" s="6" t="s">
+      <c r="C66" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D66" s="5" t="s">
+      <c r="D66" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E66" s="2" t="s">
@@ -1993,13 +1990,13 @@
       <c r="A67" s="1">
         <v>66</v>
       </c>
-      <c r="B67" s="6">
+      <c r="B67" s="5">
         <v>312938</v>
       </c>
-      <c r="C67" s="6" t="s">
+      <c r="C67" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D67" s="5" t="s">
+      <c r="D67" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E67" s="2" t="s">
@@ -2010,16 +2007,16 @@
       <c r="A68" s="1">
         <v>67</v>
       </c>
-      <c r="B68" s="6">
+      <c r="B68" s="5">
         <v>311930</v>
       </c>
-      <c r="C68" s="6" t="s">
+      <c r="C68" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D68" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E68" s="3" t="s">
+      <c r="D68" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E68" s="2" t="s">
         <v>126</v>
       </c>
     </row>
@@ -2027,16 +2024,16 @@
       <c r="A69" s="1">
         <v>68</v>
       </c>
-      <c r="B69" s="6">
+      <c r="B69" s="5">
         <v>315493</v>
       </c>
-      <c r="C69" s="6" t="s">
+      <c r="C69" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D69" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E69" s="3" t="s">
+      <c r="D69" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E69" s="2" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2044,16 +2041,16 @@
       <c r="A70" s="1">
         <v>69</v>
       </c>
-      <c r="B70" s="6">
+      <c r="B70" s="5">
         <v>313934</v>
       </c>
-      <c r="C70" s="6" t="s">
+      <c r="C70" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D70" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E70" s="3" t="s">
+      <c r="D70" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E70" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2061,16 +2058,16 @@
       <c r="A71" s="1">
         <v>70</v>
       </c>
-      <c r="B71" s="6">
+      <c r="B71" s="5">
         <v>311546</v>
       </c>
-      <c r="C71" s="6" t="s">
+      <c r="C71" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D71" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E71" s="3" t="s">
+      <c r="D71" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E71" s="2" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2078,16 +2075,16 @@
       <c r="A72" s="1">
         <v>71</v>
       </c>
-      <c r="B72" s="6">
+      <c r="B72" s="5">
         <v>315753</v>
       </c>
-      <c r="C72" s="6" t="s">
+      <c r="C72" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="D72" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E72" s="3" t="s">
+      <c r="D72" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E72" s="2" t="s">
         <v>129</v>
       </c>
     </row>
@@ -2095,16 +2092,16 @@
       <c r="A73" s="1">
         <v>72</v>
       </c>
-      <c r="B73" s="6">
+      <c r="B73" s="5">
         <v>316319</v>
       </c>
-      <c r="C73" s="6" t="s">
+      <c r="C73" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D73" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E73" s="3" t="s">
+      <c r="D73" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E73" s="2" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2112,16 +2109,16 @@
       <c r="A74" s="1">
         <v>73</v>
       </c>
-      <c r="B74" s="6">
+      <c r="B74" s="5">
         <v>315214</v>
       </c>
-      <c r="C74" s="6" t="s">
+      <c r="C74" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D74" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E74" s="3" t="s">
+      <c r="D74" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E74" s="2" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2129,16 +2126,16 @@
       <c r="A75" s="1">
         <v>74</v>
       </c>
-      <c r="B75" s="6">
+      <c r="B75" s="5">
         <v>315429</v>
       </c>
-      <c r="C75" s="6" t="s">
+      <c r="C75" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D75" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E75" s="3" t="s">
+      <c r="D75" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E75" s="2" t="s">
         <v>131</v>
       </c>
     </row>
@@ -2146,13 +2143,13 @@
       <c r="A76" s="1">
         <v>75</v>
       </c>
-      <c r="B76" s="6">
+      <c r="B76" s="5">
         <v>314455</v>
       </c>
-      <c r="C76" s="6" t="s">
+      <c r="C76" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D76" s="5" t="s">
+      <c r="D76" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E76" s="2" t="s">
@@ -2163,13 +2160,13 @@
       <c r="A77" s="1">
         <v>76</v>
       </c>
-      <c r="B77" s="6">
+      <c r="B77" s="5">
         <v>315108</v>
       </c>
-      <c r="C77" s="6" t="s">
+      <c r="C77" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D77" s="5" t="s">
+      <c r="D77" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E77" s="2" t="s">
@@ -2180,13 +2177,13 @@
       <c r="A78" s="1">
         <v>77</v>
       </c>
-      <c r="B78" s="6">
+      <c r="B78" s="5">
         <v>316243</v>
       </c>
-      <c r="C78" s="6" t="s">
+      <c r="C78" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D78" s="5" t="s">
+      <c r="D78" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E78" s="2" t="s">
@@ -2197,16 +2194,16 @@
       <c r="A79" s="1">
         <v>78</v>
       </c>
-      <c r="B79" s="6">
+      <c r="B79" s="5">
         <v>313117</v>
       </c>
-      <c r="C79" s="6" t="s">
+      <c r="C79" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D79" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E79" s="3" t="s">
+      <c r="D79" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E79" s="2" t="s">
         <v>126</v>
       </c>
     </row>
@@ -2214,16 +2211,16 @@
       <c r="A80" s="1">
         <v>79</v>
       </c>
-      <c r="B80" s="6">
+      <c r="B80" s="5">
         <v>314262</v>
       </c>
-      <c r="C80" s="6" t="s">
+      <c r="C80" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D80" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E80" s="3" t="s">
+      <c r="D80" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E80" s="2" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2231,16 +2228,16 @@
       <c r="A81" s="1">
         <v>80</v>
       </c>
-      <c r="B81" s="6">
+      <c r="B81" s="5">
         <v>314109</v>
       </c>
-      <c r="C81" s="6" t="s">
+      <c r="C81" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D81" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E81" s="3" t="s">
+      <c r="D81" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E81" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2248,16 +2245,16 @@
       <c r="A82" s="1">
         <v>81</v>
       </c>
-      <c r="B82" s="6">
+      <c r="B82" s="5">
         <v>314822</v>
       </c>
-      <c r="C82" s="6" t="s">
+      <c r="C82" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="D82" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E82" s="3" t="s">
+      <c r="D82" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E82" s="2" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2265,16 +2262,16 @@
       <c r="A83" s="1">
         <v>82</v>
       </c>
-      <c r="B83" s="6">
+      <c r="B83" s="5">
         <v>314146</v>
       </c>
-      <c r="C83" s="6" t="s">
+      <c r="C83" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D83" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E83" s="3" t="s">
+      <c r="D83" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E83" s="2" t="s">
         <v>129</v>
       </c>
     </row>
@@ -2282,16 +2279,16 @@
       <c r="A84" s="1">
         <v>83</v>
       </c>
-      <c r="B84" s="6">
+      <c r="B84" s="5">
         <v>315038</v>
       </c>
-      <c r="C84" s="6" t="s">
+      <c r="C84" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D84" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E84" s="3" t="s">
+      <c r="D84" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E84" s="2" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2299,16 +2296,16 @@
       <c r="A85" s="1">
         <v>84</v>
       </c>
-      <c r="B85" s="6">
+      <c r="B85" s="5">
         <v>316320</v>
       </c>
-      <c r="C85" s="6" t="s">
+      <c r="C85" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D85" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E85" s="3" t="s">
+      <c r="D85" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E85" s="2" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2316,16 +2313,16 @@
       <c r="A86" s="1">
         <v>85</v>
       </c>
-      <c r="B86" s="6">
+      <c r="B86" s="5">
         <v>312034</v>
       </c>
-      <c r="C86" s="6" t="s">
+      <c r="C86" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D86" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E86" s="3" t="s">
+      <c r="D86" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E86" s="2" t="s">
         <v>131</v>
       </c>
     </row>
@@ -2333,13 +2330,13 @@
       <c r="A87" s="1">
         <v>86</v>
       </c>
-      <c r="B87" s="6">
+      <c r="B87" s="5">
         <v>316323</v>
       </c>
-      <c r="C87" s="6" t="s">
+      <c r="C87" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="D87" s="5" t="s">
+      <c r="D87" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E87" s="2" t="s">
@@ -2350,13 +2347,13 @@
       <c r="A88" s="1">
         <v>87</v>
       </c>
-      <c r="B88" s="6">
+      <c r="B88" s="5">
         <v>313144</v>
       </c>
-      <c r="C88" s="6" t="s">
+      <c r="C88" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="D88" s="5" t="s">
+      <c r="D88" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E88" s="2" t="s">
@@ -2367,13 +2364,13 @@
       <c r="A89" s="1">
         <v>88</v>
       </c>
-      <c r="B89" s="6">
+      <c r="B89" s="5">
         <v>315032</v>
       </c>
-      <c r="C89" s="6" t="s">
+      <c r="C89" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="D89" s="5" t="s">
+      <c r="D89" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E89" s="2" t="s">
@@ -2384,16 +2381,16 @@
       <c r="A90" s="1">
         <v>89</v>
       </c>
-      <c r="B90" s="6">
+      <c r="B90" s="5">
         <v>316325</v>
       </c>
-      <c r="C90" s="6" t="s">
+      <c r="C90" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D90" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E90" s="3" t="s">
+      <c r="D90" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E90" s="2" t="s">
         <v>126</v>
       </c>
     </row>
@@ -2401,16 +2398,16 @@
       <c r="A91" s="1">
         <v>90</v>
       </c>
-      <c r="B91" s="6">
+      <c r="B91" s="5">
         <v>316315</v>
       </c>
-      <c r="C91" s="6" t="s">
+      <c r="C91" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="D91" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E91" s="3" t="s">
+      <c r="D91" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E91" s="2" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2418,16 +2415,16 @@
       <c r="A92" s="1">
         <v>91</v>
       </c>
-      <c r="B92" s="6">
+      <c r="B92" s="5">
         <v>314379</v>
       </c>
-      <c r="C92" s="6" t="s">
+      <c r="C92" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D92" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E92" s="3" t="s">
+      <c r="D92" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E92" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2435,16 +2432,16 @@
       <c r="A93" s="1">
         <v>92</v>
       </c>
-      <c r="B93" s="6">
+      <c r="B93" s="5">
         <v>316321</v>
       </c>
-      <c r="C93" s="6" t="s">
+      <c r="C93" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D93" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E93" s="3" t="s">
+      <c r="D93" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E93" s="2" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2452,16 +2449,16 @@
       <c r="A94" s="1">
         <v>93</v>
       </c>
-      <c r="B94" s="6">
+      <c r="B94" s="5">
         <v>314205</v>
       </c>
-      <c r="C94" s="6" t="s">
+      <c r="C94" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="D94" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E94" s="3" t="s">
+      <c r="D94" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E94" s="2" t="s">
         <v>129</v>
       </c>
     </row>
@@ -2469,16 +2466,16 @@
       <c r="A95" s="1">
         <v>94</v>
       </c>
-      <c r="B95" s="6">
+      <c r="B95" s="5">
         <v>315236</v>
       </c>
-      <c r="C95" s="6" t="s">
+      <c r="C95" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D95" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E95" s="3" t="s">
+      <c r="D95" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E95" s="2" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2486,16 +2483,16 @@
       <c r="A96" s="1">
         <v>95</v>
       </c>
-      <c r="B96" s="6">
+      <c r="B96" s="5">
         <v>315039</v>
       </c>
-      <c r="C96" s="6" t="s">
+      <c r="C96" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="D96" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E96" s="3" t="s">
+      <c r="D96" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E96" s="2" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2503,16 +2500,16 @@
       <c r="A97" s="1">
         <v>96</v>
       </c>
-      <c r="B97" s="6">
+      <c r="B97" s="5">
         <v>314206</v>
       </c>
-      <c r="C97" s="6" t="s">
+      <c r="C97" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="D97" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E97" s="3" t="s">
+      <c r="D97" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E97" s="2" t="s">
         <v>131</v>
       </c>
     </row>
@@ -2520,13 +2517,13 @@
       <c r="A98" s="1">
         <v>97</v>
       </c>
-      <c r="B98" s="6">
+      <c r="B98" s="5">
         <v>313888</v>
       </c>
-      <c r="C98" s="6" t="s">
+      <c r="C98" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="D98" s="5" t="s">
+      <c r="D98" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E98" s="2" t="s">
@@ -2537,13 +2534,13 @@
       <c r="A99" s="1">
         <v>98</v>
       </c>
-      <c r="B99" s="6">
+      <c r="B99" s="5">
         <v>316784</v>
       </c>
-      <c r="C99" s="6" t="s">
+      <c r="C99" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="D99" s="5" t="s">
+      <c r="D99" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E99" s="2" t="s">
@@ -2554,13 +2551,13 @@
       <c r="A100" s="1">
         <v>99</v>
       </c>
-      <c r="B100" s="6">
+      <c r="B100" s="5">
         <v>315594</v>
       </c>
-      <c r="C100" s="6" t="s">
+      <c r="C100" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="D100" s="5" t="s">
+      <c r="D100" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E100" s="2" t="s">
@@ -2571,16 +2568,16 @@
       <c r="A101" s="1">
         <v>100</v>
       </c>
-      <c r="B101" s="6">
+      <c r="B101" s="5">
         <v>316324</v>
       </c>
-      <c r="C101" s="6" t="s">
+      <c r="C101" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="D101" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E101" s="3" t="s">
+      <c r="D101" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E101" s="2" t="s">
         <v>126</v>
       </c>
     </row>
@@ -2588,16 +2585,16 @@
       <c r="A102" s="1">
         <v>101</v>
       </c>
-      <c r="B102" s="6">
+      <c r="B102" s="5">
         <v>316173</v>
       </c>
-      <c r="C102" s="6" t="s">
+      <c r="C102" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="D102" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E102" s="3" t="s">
+      <c r="D102" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E102" s="2" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2605,16 +2602,16 @@
       <c r="A103" s="1">
         <v>102</v>
       </c>
-      <c r="B103" s="6">
+      <c r="B103" s="5">
         <v>315034</v>
       </c>
-      <c r="C103" s="6" t="s">
+      <c r="C103" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="D103" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E103" s="3" t="s">
+      <c r="D103" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E103" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2622,16 +2619,16 @@
       <c r="A104" s="1">
         <v>103</v>
       </c>
-      <c r="B104" s="6">
+      <c r="B104" s="5">
         <v>315761</v>
       </c>
-      <c r="C104" s="6" t="s">
+      <c r="C104" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="D104" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E104" s="3" t="s">
+      <c r="D104" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E104" s="2" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2639,16 +2636,16 @@
       <c r="A105" s="1">
         <v>104</v>
       </c>
-      <c r="B105" s="6">
+      <c r="B105" s="5">
         <v>314099</v>
       </c>
-      <c r="C105" s="6" t="s">
+      <c r="C105" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="D105" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E105" s="3" t="s">
+      <c r="D105" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E105" s="2" t="s">
         <v>129</v>
       </c>
     </row>
@@ -2656,16 +2653,16 @@
       <c r="A106" s="1">
         <v>105</v>
       </c>
-      <c r="B106" s="6">
+      <c r="B106" s="5">
         <v>314114</v>
       </c>
-      <c r="C106" s="6" t="s">
+      <c r="C106" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="D106" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E106" s="3" t="s">
+      <c r="D106" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E106" s="2" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2673,16 +2670,16 @@
       <c r="A107" s="1">
         <v>106</v>
       </c>
-      <c r="B107" s="6">
+      <c r="B107" s="5">
         <v>314204</v>
       </c>
-      <c r="C107" s="6" t="s">
+      <c r="C107" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="D107" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E107" s="3" t="s">
+      <c r="D107" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E107" s="2" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2690,16 +2687,16 @@
       <c r="A108" s="1">
         <v>107</v>
       </c>
-      <c r="B108" s="6">
+      <c r="B108" s="5">
         <v>314218</v>
       </c>
-      <c r="C108" s="6" t="s">
+      <c r="C108" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="D108" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E108" s="3" t="s">
+      <c r="D108" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E108" s="2" t="s">
         <v>131</v>
       </c>
     </row>
@@ -2707,13 +2704,13 @@
       <c r="A109" s="1">
         <v>108</v>
       </c>
-      <c r="B109" s="6">
+      <c r="B109" s="5">
         <v>314472</v>
       </c>
-      <c r="C109" s="6" t="s">
+      <c r="C109" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="D109" s="5" t="s">
+      <c r="D109" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E109" s="2" t="s">
@@ -2724,13 +2721,13 @@
       <c r="A110" s="1">
         <v>109</v>
       </c>
-      <c r="B110" s="6">
+      <c r="B110" s="5">
         <v>315636</v>
       </c>
-      <c r="C110" s="6" t="s">
+      <c r="C110" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="D110" s="5" t="s">
+      <c r="D110" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E110" s="2" t="s">
@@ -2741,13 +2738,13 @@
       <c r="A111" s="1">
         <v>110</v>
       </c>
-      <c r="B111" s="6">
+      <c r="B111" s="5">
         <v>314115</v>
       </c>
-      <c r="C111" s="6" t="s">
+      <c r="C111" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="D111" s="5" t="s">
+      <c r="D111" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E111" s="2" t="s">
@@ -2758,16 +2755,16 @@
       <c r="A112" s="1">
         <v>111</v>
       </c>
-      <c r="B112" s="6">
+      <c r="B112" s="5">
         <v>314110</v>
       </c>
-      <c r="C112" s="6" t="s">
+      <c r="C112" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="D112" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E112" s="3" t="s">
+      <c r="D112" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E112" s="2" t="s">
         <v>126</v>
       </c>
     </row>
@@ -2775,16 +2772,16 @@
       <c r="A113" s="1">
         <v>112</v>
       </c>
-      <c r="B113" s="6">
+      <c r="B113" s="5">
         <v>314729</v>
       </c>
-      <c r="C113" s="6" t="s">
+      <c r="C113" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="D113" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E113" s="3" t="s">
+      <c r="D113" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E113" s="2" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2792,16 +2789,16 @@
       <c r="A114" s="1">
         <v>113</v>
       </c>
-      <c r="B114" s="6">
+      <c r="B114" s="5">
         <v>316322</v>
       </c>
-      <c r="C114" s="6" t="s">
+      <c r="C114" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="D114" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E114" s="3" t="s">
+      <c r="D114" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E114" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2809,16 +2806,16 @@
       <c r="A115" s="1">
         <v>114</v>
       </c>
-      <c r="B115" s="6">
+      <c r="B115" s="5">
         <v>315658</v>
       </c>
-      <c r="C115" s="6" t="s">
+      <c r="C115" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="D115" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E115" s="3" t="s">
+      <c r="D115" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E115" s="2" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2826,16 +2823,16 @@
       <c r="A116" s="1">
         <v>115</v>
       </c>
-      <c r="B116" s="6">
+      <c r="B116" s="5">
         <v>314209</v>
       </c>
-      <c r="C116" s="6" t="s">
+      <c r="C116" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="D116" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E116" s="3" t="s">
+      <c r="D116" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E116" s="2" t="s">
         <v>129</v>
       </c>
     </row>
@@ -2843,16 +2840,16 @@
       <c r="A117" s="1">
         <v>116</v>
       </c>
-      <c r="B117" s="6">
+      <c r="B117" s="5">
         <v>311841</v>
       </c>
-      <c r="C117" s="6" t="s">
+      <c r="C117" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="D117" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E117" s="3" t="s">
+      <c r="D117" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E117" s="2" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2860,16 +2857,16 @@
       <c r="A118" s="1">
         <v>117</v>
       </c>
-      <c r="B118" s="6">
+      <c r="B118" s="5">
         <v>313283</v>
       </c>
-      <c r="C118" s="6" t="s">
+      <c r="C118" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="D118" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E118" s="3" t="s">
+      <c r="D118" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E118" s="2" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2877,16 +2874,16 @@
       <c r="A119" s="1">
         <v>118</v>
       </c>
-      <c r="B119" s="6">
+      <c r="B119" s="5">
         <v>316734</v>
       </c>
-      <c r="C119" s="6" t="s">
+      <c r="C119" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="D119" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E119" s="3" t="s">
+      <c r="D119" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E119" s="2" t="s">
         <v>131</v>
       </c>
     </row>

</xml_diff>